<commit_message>
Add Planning Court in London Administrative Court
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/london-administrative-court-daily-cause-list/londonAdministrativeCourtDailyCauseList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/london-administrative-court-daily-cause-list/londonAdministrativeCourtDailyCauseList.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kian.kwa/IdeaProjects/pip-data-management/src/integrationTest/resources/data/non-strategic/london-administrative-court-daily-cause-list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junaid.iqbal/Documents/GitHub/pip-data-management/src/integrationTest/resources/data/non-strategic/london-administrative-court-daily-cause-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8804B630-6454-714A-B29D-69D178762227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AF0814-15BD-2C42-A834-F49A4A4169A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53800" yWindow="2820" windowWidth="27640" windowHeight="16880" xr2:uid="{E584EC2B-A09C-FB4D-91FD-7FFB366A043F}"/>
+    <workbookView xWindow="-31900" yWindow="-400" windowWidth="30240" windowHeight="17400" xr2:uid="{E584EC2B-A09C-FB4D-91FD-7FFB366A043F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hearing list" sheetId="2" r:id="rId1"/>
+    <sheet name="Planning court" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>Venue</t>
   </si>
@@ -463,10 +464,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E2CE13-B4D6-874A-98F8-EA0522D886FF}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="37.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>12345</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>12346</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846C4FC4-FD65-1D43-90C9-25FA31CE686A}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change the sheet name
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/london-administrative-court-daily-cause-list/londonAdministrativeCourtDailyCauseList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/london-administrative-court-daily-cause-list/londonAdministrativeCourtDailyCauseList.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junaid.iqbal/Documents/GitHub/pip-data-management/src/integrationTest/resources/data/non-strategic/london-administrative-court-daily-cause-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AF0814-15BD-2C42-A834-F49A4A4169A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471B4B9B-E8BE-5745-8704-3D404A167A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31900" yWindow="-400" windowWidth="30240" windowHeight="17400" xr2:uid="{E584EC2B-A09C-FB4D-91FD-7FFB366A043F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hearing list" sheetId="2" r:id="rId1"/>
+    <sheet name="London administrative court" sheetId="2" r:id="rId1"/>
     <sheet name="Planning court" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -468,7 +468,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
PUB-2917 Add Planning Court in London Administrative Court (#736)
* Add Planning Court in London Administrative Court

* change the sheet name

* remove not needed column

---------

Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/london-administrative-court-daily-cause-list/londonAdministrativeCourtDailyCauseList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/london-administrative-court-daily-cause-list/londonAdministrativeCourtDailyCauseList.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kian.kwa/IdeaProjects/pip-data-management/src/integrationTest/resources/data/non-strategic/london-administrative-court-daily-cause-list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junaid.iqbal/Documents/GitHub/pip-data-management/src/integrationTest/resources/data/non-strategic/london-administrative-court-daily-cause-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8804B630-6454-714A-B29D-69D178762227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471B4B9B-E8BE-5745-8704-3D404A167A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53800" yWindow="2820" windowWidth="27640" windowHeight="16880" xr2:uid="{E584EC2B-A09C-FB4D-91FD-7FFB366A043F}"/>
+    <workbookView xWindow="-31900" yWindow="-400" windowWidth="30240" windowHeight="17400" xr2:uid="{E584EC2B-A09C-FB4D-91FD-7FFB366A043F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="London administrative court" sheetId="2" r:id="rId1"/>
+    <sheet name="Planning court" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>Venue</t>
   </si>
@@ -463,10 +464,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E2CE13-B4D6-874A-98F8-EA0522D886FF}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="37.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>12345</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>12346</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846C4FC4-FD65-1D43-90C9-25FA31CE686A}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>

</xml_diff>